<commit_message>
WIP: Highest level documentation of data
</commit_message>
<xml_diff>
--- a/DatasetConfiguration/DatasetDefinition1.xlsx
+++ b/DatasetConfiguration/DatasetDefinition1.xlsx
@@ -5,19 +5,25 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet 2" sheetId="2" r:id="rId5"/>
+    <sheet name="BuildingInfoTable" sheetId="1" r:id="rId4"/>
+    <sheet name="ExtraFeaturesTable" sheetId="2" r:id="rId5"/>
+    <sheet name="OwnerInfoTable" sheetId="3" r:id="rId6"/>
+    <sheet name="ParcelSummaryTable" sheetId="4" r:id="rId7"/>
+    <sheet name="SalesTable" sheetId="5" r:id="rId8"/>
+    <sheet name="SketchesTable" sheetId="6" r:id="rId9"/>
+    <sheet name="TaxCollectorTable" sheetId="7" r:id="rId10"/>
+    <sheet name="ValuationTable" sheetId="8" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
   <si>
     <t>BuildingInfoTable</t>
   </si>
   <si>
-    <t>id</t>
+    <t>DATA SOURCE</t>
   </si>
   <si>
     <t>type</t>
@@ -68,7 +74,181 @@
     <t>effectiveYearBuilt</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <t>SQlite</t>
+  </si>
+  <si>
+    <t>OpenSearch Database</t>
+  </si>
+  <si>
+    <t>Hugging Face Dataset #</t>
+  </si>
+  <si>
+    <t>ReGrid API</t>
+  </si>
+  <si>
+    <t>ExtraFeaturesTable</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>lengthWidth</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>yearBuilt</t>
+  </si>
+  <si>
+    <t>OwnerInfoTable</t>
+  </si>
+  <si>
+    <t>contactName</t>
+  </si>
+  <si>
+    <t>streetAddress</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>ParcelSummaryTable</t>
+  </si>
+  <si>
+    <t>parcelId</t>
+  </si>
+  <si>
+    <t>parcelAddress</t>
+  </si>
+  <si>
+    <t>propertyUseCode</t>
+  </si>
+  <si>
+    <t>acreage</t>
+  </si>
+  <si>
+    <t>homestead</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>gpsPolygonCoordinates</t>
+  </si>
+  <si>
+    <t>altParcelId1</t>
+  </si>
+  <si>
+    <t>altParcelId2</t>
+  </si>
+  <si>
+    <t>SalesTable</t>
+  </si>
+  <si>
+    <t>multiParcel</t>
+  </si>
+  <si>
+    <t>salePrice</t>
+  </si>
+  <si>
+    <t>instrument</t>
+  </si>
+  <si>
+    <t>bookPage</t>
+  </si>
+  <si>
+    <t>qualification</t>
+  </si>
+  <si>
+    <t>vacantOrImproved</t>
+  </si>
+  <si>
+    <t>saleDate</t>
+  </si>
+  <si>
+    <t>grantee</t>
+  </si>
+  <si>
+    <t>grantor</t>
+  </si>
+  <si>
+    <t>SketchesTable</t>
+  </si>
+  <si>
+    <t>pngFilename</t>
+  </si>
+  <si>
+    <t>TaxCollectorTable</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>ValuationTable</t>
+  </si>
+  <si>
+    <t>buildingValue</t>
+  </si>
+  <si>
+    <t>extraFeaturesValue</t>
+  </si>
+  <si>
+    <t>landValue</t>
+  </si>
+  <si>
+    <t>landAgriculturalValue</t>
+  </si>
+  <si>
+    <t>justMarketValue</t>
+  </si>
+  <si>
+    <t>assessedValue</t>
+  </si>
+  <si>
+    <t>exemptValue</t>
+  </si>
+  <si>
+    <t>taxableValue</t>
+  </si>
+  <si>
+    <t>maximumSaveOurHomesPortability</t>
+  </si>
+  <si>
+    <t>justvalhomestead</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>lnd_val</t>
+  </si>
+  <si>
+    <t>asvalagval</t>
+  </si>
+  <si>
+    <t>parval</t>
+  </si>
+  <si>
+    <t>assedvalschool</t>
+  </si>
+  <si>
+    <t>assedvalnonschool</t>
+  </si>
+  <si>
+    <t>taxvalschool</t>
   </si>
 </sst>
 </file>
@@ -96,7 +276,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +298,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -241,7 +427,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -254,10 +440,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -266,7 +452,7 @@
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -275,11 +461,41 @@
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -298,11 +514,12 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ff919191"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="fffff056"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="fffefffe"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1331,7 +1548,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:Q25"/>
+  <dimension ref="A2:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1339,7 +1556,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="17" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7891" style="1" customWidth="1"/>
+    <col min="2" max="17" width="16.3516" style="1" customWidth="1"/>
     <col min="18" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1418,7 +1636,9 @@
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="5"/>
+      <c r="A3" t="s" s="5">
+        <v>18</v>
+      </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1437,7 +1657,9 @@
       <c r="Q3" s="7"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="8"/>
+      <c r="A4" t="s" s="8">
+        <v>19</v>
+      </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1456,7 +1678,9 @@
       <c r="Q4" s="10"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="8"/>
+      <c r="A5" t="s" s="8">
+        <v>20</v>
+      </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -1475,7 +1699,9 @@
       <c r="Q5" s="10"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="8"/>
+      <c r="A6" t="s" s="8">
+        <v>21</v>
+      </c>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -1494,7 +1720,7 @@
       <c r="Q6" s="10"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -1513,7 +1739,7 @@
       <c r="Q7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="8"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -1532,7 +1758,7 @@
       <c r="Q8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="8"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -1551,7 +1777,7 @@
       <c r="Q9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="8"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -1570,7 +1796,7 @@
       <c r="Q10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="8"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -1589,7 +1815,7 @@
       <c r="Q11" s="10"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="8"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1608,7 +1834,7 @@
       <c r="Q12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="8"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -1627,7 +1853,7 @@
       <c r="Q13" s="10"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="8"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1646,7 +1872,7 @@
       <c r="Q14" s="10"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="8"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -1665,7 +1891,7 @@
       <c r="Q15" s="10"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="8"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -1684,7 +1910,7 @@
       <c r="Q16" s="10"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="8"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -1703,7 +1929,7 @@
       <c r="Q17" s="10"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="8"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1722,7 +1948,7 @@
       <c r="Q18" s="10"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="8"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1741,7 +1967,7 @@
       <c r="Q19" s="10"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="8"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1760,7 +1986,7 @@
       <c r="Q20" s="10"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="8"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1779,7 +2005,7 @@
       <c r="Q21" s="10"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="8"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1798,7 +2024,7 @@
       <c r="Q22" s="10"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="8"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -1817,7 +2043,7 @@
       <c r="Q23" s="10"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="8"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -1836,7 +2062,7 @@
       <c r="Q24" s="10"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="8"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -1853,6 +2079,44 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
+    </row>
+    <row r="26" ht="20.05" customHeight="1">
+      <c r="A26" s="11"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
+      <c r="A27" s="11"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1871,7 +2135,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E11"/>
+  <dimension ref="A2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1879,92 +2143,1058 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="11" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="12" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s" s="4">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="5"/>
+      <c r="A3" t="s" s="5">
+        <v>18</v>
+      </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="8"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="A4" t="s" s="8">
+        <v>19</v>
+      </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="8"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="A5" t="s" s="8">
+        <v>20</v>
+      </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="8"/>
+      <c r="A6" t="s" s="8">
+        <v>21</v>
+      </c>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="8"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="8"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="8"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="8"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="7" width="16.3516" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="A4" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="A5" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="11" width="16.3516" style="14" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="A4" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="A5" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="1.17188" style="15" customWidth="1"/>
+    <col min="2" max="11" width="16.3516" style="15" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="B1" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="B2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s" s="4">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s" s="4">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s" s="4">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s" s="4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="B3" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="B4" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="B5" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="B6" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="B7" s="11"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="B8" s="11"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="B9" s="11"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="B10" s="11"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="B11" s="11"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="2" width="16.3516" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="16.3516" style="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="A4" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="A5" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="B5" s="9"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="2" width="16.3516" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="16.3516" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="18">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="A4" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="A5" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="B5" s="9"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="2" width="16.3516" style="19" customWidth="1"/>
+    <col min="3" max="3" width="18.3672" style="19" customWidth="1"/>
+    <col min="4" max="7" width="16.3516" style="19" customWidth="1"/>
+    <col min="8" max="8" width="17.6406" style="19" customWidth="1"/>
+    <col min="9" max="10" width="16.3516" style="19" customWidth="1"/>
+    <col min="11" max="16384" width="16.3516" style="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" ht="32.25" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s" s="4">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s" s="4">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s" s="4">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="I2" t="s" s="4">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="A4" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="A5" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s" s="20">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s" s="21">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s" s="22">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s" s="22">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s" s="22">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s" s="22">
+        <v>74</v>
+      </c>
+      <c r="H6" t="s" s="21">
+        <v>75</v>
+      </c>
+      <c r="I6" t="s" s="22">
+        <v>76</v>
+      </c>
+      <c r="J6" t="s" s="21">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>